<commit_message>
Use multiple ranges for print area.
</commit_message>
<xml_diff>
--- a/openpyxl/packaging/tests/data/print_settings.xlsx
+++ b/openpyxl/packaging/tests/data/print_settings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18480" tabRatio="500"/>
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet!$A$1:$D$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet!$A$1:$D$5,Sheet!$B$9:$F$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet!$1:$1</definedName>
     <definedName name="name">"charlie"</definedName>
     <definedName name="pi">41699</definedName>

</xml_diff>